<commit_message>
updated IFNA in assignment 7
</commit_message>
<xml_diff>
--- a/Assignment 7 WPS.xlsx
+++ b/Assignment 7 WPS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\2. June\22\File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\2. June\22\Assignments_6_7_8\practice_exercise_6_7_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640CCBA2-E4B6-4425-BFC7-A9C7B3D5D5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C173E5E1-980D-43C8-92DA-3C805A1B8D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -370,7 +370,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -426,9 +426,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1173,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I152" sqref="I152"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L124" sqref="L124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -5952,7 +5949,7 @@
         <v>10</v>
       </c>
       <c r="I123" s="11">
-        <f>D123*VLOOKUP(D123,$B$144:$C$148,2)</f>
+        <f>_xlfn.IFNA(D123*VLOOKUP(D123,$B$144:$C$148,2),0)</f>
         <v>173.59580000000003</v>
       </c>
       <c r="J123" s="14"/>
@@ -5993,7 +5990,7 @@
         <v>11</v>
       </c>
       <c r="I124" s="11">
-        <f t="shared" ref="I124:I142" si="5">D124*VLOOKUP(D124,$B$144:$C$148,2)</f>
+        <f t="shared" ref="I124:I142" si="5">_xlfn.IFNA(D124*VLOOKUP(D124,$B$144:$C$148,2),0)</f>
         <v>121.30930000000001</v>
       </c>
       <c r="J124" s="14"/>
@@ -6279,9 +6276,9 @@
       <c r="H131" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I131" s="11" t="e">
-        <f>D131*VLOOKUP(D131,$B$144:$C$148,2)</f>
-        <v>#N/A</v>
+      <c r="I131" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="J131" s="14"/>
       <c r="K131" s="1"/>
@@ -6361,9 +6358,9 @@
       <c r="H133" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I133" s="11" t="e">
+      <c r="I133" s="11">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J133" s="14"/>
       <c r="K133" s="1"/>
@@ -6402,9 +6399,9 @@
       <c r="H134" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I134" s="11" t="e">
+      <c r="I134" s="11">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J134" s="14"/>
       <c r="K134" s="1"/>
@@ -6443,9 +6440,9 @@
       <c r="H135" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I135" s="11" t="e">
+      <c r="I135" s="11">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J135" s="14"/>
       <c r="K135" s="1"/>
@@ -6484,9 +6481,9 @@
       <c r="H136" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I136" s="11" t="e">
+      <c r="I136" s="11">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J136" s="14"/>
       <c r="K136" s="1"/>
@@ -6525,9 +6522,9 @@
       <c r="H137" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I137" s="11" t="e">
+      <c r="I137" s="11">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J137" s="14"/>
       <c r="K137" s="1"/>
@@ -6607,9 +6604,9 @@
       <c r="H139" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I139" s="11" t="e">
+      <c r="I139" s="11">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J139" s="14"/>
       <c r="K139" s="1"/>
@@ -6648,9 +6645,9 @@
       <c r="H140" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I140" s="11" t="e">
+      <c r="I140" s="11">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J140" s="14"/>
       <c r="K140" s="1"/>
@@ -8039,7 +8036,7 @@
       <c r="H181" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I181" s="19" cm="1">
+      <c r="I181" s="11" cm="1">
         <f t="array" ref="I181">_xlfn.IFNA(_xlfn.IFS($D181&gt;=$B$206,$D181*0.15,AND($D181&lt;$B$206,$D181&gt;=$B$205),$D181*0.07,AND($D181&lt;$B$205,$D181&gt;=$B$204),$D181*0.03,AND($D181&lt;$B$204,$D181&gt;=$B$203),D181*0.01),0)</f>
         <v>173.59580000000003</v>
       </c>
@@ -8080,7 +8077,7 @@
       <c r="H182" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I182" s="19" cm="1">
+      <c r="I182" s="11" cm="1">
         <f t="array" ref="I182">_xlfn.IFNA(_xlfn.IFS($D182&gt;=$B$206,$D182*0.15,AND($D182&lt;$B$206,$D182&gt;=$B$205),$D182*0.07,AND($D182&lt;$B$205,$D182&gt;=$B$204),$D182*0.03,AND($D182&lt;$B$204,$D182&gt;=$B$203),D182*0.01),0)</f>
         <v>121.30930000000001</v>
       </c>
@@ -8121,7 +8118,7 @@
       <c r="H183" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I183" s="19" cm="1">
+      <c r="I183" s="11" cm="1">
         <f t="array" ref="I183">_xlfn.IFNA(_xlfn.IFS($D183&gt;=$B$206,$D183*0.15,AND($D183&lt;$B$206,$D183&gt;=$B$205),$D183*0.07,AND($D183&lt;$B$205,$D183&gt;=$B$204),$D183*0.03,AND($D183&lt;$B$204,$D183&gt;=$B$203),D183*0.01),0)</f>
         <v>11.7499</v>
       </c>
@@ -8162,7 +8159,7 @@
       <c r="H184" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I184" s="19" cm="1">
+      <c r="I184" s="11" cm="1">
         <f t="array" ref="I184">_xlfn.IFNA(_xlfn.IFS($D184&gt;=$B$206,$D184*0.15,AND($D184&lt;$B$206,$D184&gt;=$B$205),$D184*0.07,AND($D184&lt;$B$205,$D184&gt;=$B$204),$D184*0.03,AND($D184&lt;$B$204,$D184&gt;=$B$203),D184*0.01),0)</f>
         <v>125.99930000000002</v>
       </c>
@@ -8203,7 +8200,7 @@
       <c r="H185" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I185" s="19" cm="1">
+      <c r="I185" s="11" cm="1">
         <f t="array" ref="I185">_xlfn.IFNA(_xlfn.IFS($D185&gt;=$B$206,$D185*0.15,AND($D185&lt;$B$206,$D185&gt;=$B$205),$D185*0.07,AND($D185&lt;$B$205,$D185&gt;=$B$204),$D185*0.03,AND($D185&lt;$B$204,$D185&gt;=$B$203),D185*0.01),0)</f>
         <v>474.74849999999992</v>
       </c>
@@ -8244,7 +8241,7 @@
       <c r="H186" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I186" s="19" cm="1">
+      <c r="I186" s="11" cm="1">
         <f t="array" ref="I186">_xlfn.IFNA(_xlfn.IFS($D186&gt;=$B$206,$D186*0.15,AND($D186&lt;$B$206,$D186&gt;=$B$205),$D186*0.07,AND($D186&lt;$B$205,$D186&gt;=$B$204),$D186*0.03,AND($D186&lt;$B$204,$D186&gt;=$B$203),D186*0.01),0)</f>
         <v>11.99</v>
       </c>
@@ -8285,7 +8282,7 @@
       <c r="H187" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I187" s="19" cm="1">
+      <c r="I187" s="11" cm="1">
         <f t="array" ref="I187">_xlfn.IFNA(_xlfn.IFS($D187&gt;=$B$206,$D187*0.15,AND($D187&lt;$B$206,$D187&gt;=$B$205),$D187*0.07,AND($D187&lt;$B$205,$D187&gt;=$B$204),$D187*0.03,AND($D187&lt;$B$204,$D187&gt;=$B$203),D187*0.01),0)</f>
         <v>6.9995000000000003</v>
       </c>
@@ -8326,7 +8323,7 @@
       <c r="H188" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I188" s="19" cm="1">
+      <c r="I188" s="11" cm="1">
         <f t="array" ref="I188">_xlfn.IFNA(_xlfn.IFS($D188&gt;=$B$206,$D188*0.15,AND($D188&lt;$B$206,$D188&gt;=$B$205),$D188*0.07,AND($D188&lt;$B$205,$D188&gt;=$B$204),$D188*0.03,AND($D188&lt;$B$204,$D188&gt;=$B$203),D188*0.01),0)</f>
         <v>9.49</v>
       </c>
@@ -8367,7 +8364,7 @@
       <c r="H189" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I189" s="19" cm="1">
+      <c r="I189" s="11" cm="1">
         <f t="array" ref="I189">_xlfn.IFNA(_xlfn.IFS($D189&gt;=$B$206,$D189*0.15,AND($D189&lt;$B$206,$D189&gt;=$B$205),$D189*0.07,AND($D189&lt;$B$205,$D189&gt;=$B$204),$D189*0.03,AND($D189&lt;$B$204,$D189&gt;=$B$203),D189*0.01),0)</f>
         <v>0</v>
       </c>
@@ -8408,7 +8405,7 @@
       <c r="H190" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I190" s="19" cm="1">
+      <c r="I190" s="11" cm="1">
         <f t="array" ref="I190">_xlfn.IFNA(_xlfn.IFS($D190&gt;=$B$206,$D190*0.15,AND($D190&lt;$B$206,$D190&gt;=$B$205),$D190*0.07,AND($D190&lt;$B$205,$D190&gt;=$B$204),$D190*0.03,AND($D190&lt;$B$204,$D190&gt;=$B$203),D190*0.01),0)</f>
         <v>45.75</v>
       </c>
@@ -8449,7 +8446,7 @@
       <c r="H191" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I191" s="19" cm="1">
+      <c r="I191" s="11" cm="1">
         <f t="array" ref="I191">_xlfn.IFNA(_xlfn.IFS($D191&gt;=$B$206,$D191*0.15,AND($D191&lt;$B$206,$D191&gt;=$B$205),$D191*0.07,AND($D191&lt;$B$205,$D191&gt;=$B$204),$D191*0.03,AND($D191&lt;$B$204,$D191&gt;=$B$203),D191*0.01),0)</f>
         <v>0</v>
       </c>
@@ -8490,7 +8487,7 @@
       <c r="H192" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I192" s="19" cm="1">
+      <c r="I192" s="11" cm="1">
         <f t="array" ref="I192">_xlfn.IFNA(_xlfn.IFS($D192&gt;=$B$206,$D192*0.15,AND($D192&lt;$B$206,$D192&gt;=$B$205),$D192*0.07,AND($D192&lt;$B$205,$D192&gt;=$B$204),$D192*0.03,AND($D192&lt;$B$204,$D192&gt;=$B$203),D192*0.01),0)</f>
         <v>0</v>
       </c>
@@ -8531,7 +8528,7 @@
       <c r="H193" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I193" s="19" cm="1">
+      <c r="I193" s="11" cm="1">
         <f t="array" ref="I193">_xlfn.IFNA(_xlfn.IFS($D193&gt;=$B$206,$D193*0.15,AND($D193&lt;$B$206,$D193&gt;=$B$205),$D193*0.07,AND($D193&lt;$B$205,$D193&gt;=$B$204),$D193*0.03,AND($D193&lt;$B$204,$D193&gt;=$B$203),D193*0.01),0)</f>
         <v>0</v>
       </c>
@@ -8572,7 +8569,7 @@
       <c r="H194" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I194" s="19" cm="1">
+      <c r="I194" s="11" cm="1">
         <f t="array" ref="I194">_xlfn.IFNA(_xlfn.IFS($D194&gt;=$B$206,$D194*0.15,AND($D194&lt;$B$206,$D194&gt;=$B$205),$D194*0.07,AND($D194&lt;$B$205,$D194&gt;=$B$204),$D194*0.03,AND($D194&lt;$B$204,$D194&gt;=$B$203),D194*0.01),0)</f>
         <v>0</v>
       </c>
@@ -8613,7 +8610,7 @@
       <c r="H195" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I195" s="19" cm="1">
+      <c r="I195" s="11" cm="1">
         <f t="array" ref="I195">_xlfn.IFNA(_xlfn.IFS($D195&gt;=$B$206,$D195*0.15,AND($D195&lt;$B$206,$D195&gt;=$B$205),$D195*0.07,AND($D195&lt;$B$205,$D195&gt;=$B$204),$D195*0.03,AND($D195&lt;$B$204,$D195&gt;=$B$203),D195*0.01),0)</f>
         <v>0</v>
       </c>
@@ -8654,7 +8651,7 @@
       <c r="H196" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I196" s="19" cm="1">
+      <c r="I196" s="11" cm="1">
         <f t="array" ref="I196">_xlfn.IFNA(_xlfn.IFS($D196&gt;=$B$206,$D196*0.15,AND($D196&lt;$B$206,$D196&gt;=$B$205),$D196*0.07,AND($D196&lt;$B$205,$D196&gt;=$B$204),$D196*0.03,AND($D196&lt;$B$204,$D196&gt;=$B$203),D196*0.01),0)</f>
         <v>125.99930000000002</v>
       </c>
@@ -8695,7 +8692,7 @@
       <c r="H197" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I197" s="19" cm="1">
+      <c r="I197" s="11" cm="1">
         <f t="array" ref="I197">_xlfn.IFNA(_xlfn.IFS($D197&gt;=$B$206,$D197*0.15,AND($D197&lt;$B$206,$D197&gt;=$B$205),$D197*0.07,AND($D197&lt;$B$205,$D197&gt;=$B$204),$D197*0.03,AND($D197&lt;$B$204,$D197&gt;=$B$203),D197*0.01),0)</f>
         <v>0</v>
       </c>
@@ -8736,7 +8733,7 @@
       <c r="H198" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I198" s="19" cm="1">
+      <c r="I198" s="11" cm="1">
         <f t="array" ref="I198">_xlfn.IFNA(_xlfn.IFS($D198&gt;=$B$206,$D198*0.15,AND($D198&lt;$B$206,$D198&gt;=$B$205),$D198*0.07,AND($D198&lt;$B$205,$D198&gt;=$B$204),$D198*0.03,AND($D198&lt;$B$204,$D198&gt;=$B$203),D198*0.01),0)</f>
         <v>0</v>
       </c>
@@ -8777,7 +8774,7 @@
       <c r="H199" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I199" s="19" cm="1">
+      <c r="I199" s="11" cm="1">
         <f t="array" ref="I199">_xlfn.IFNA(_xlfn.IFS($D199&gt;=$B$206,$D199*0.15,AND($D199&lt;$B$206,$D199&gt;=$B$205),$D199*0.07,AND($D199&lt;$B$205,$D199&gt;=$B$204),$D199*0.03,AND($D199&lt;$B$204,$D199&gt;=$B$203),D199*0.01),0)</f>
         <v>5.6000000000000005</v>
       </c>
@@ -8818,7 +8815,7 @@
       <c r="H200" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I200" s="19" cm="1">
+      <c r="I200" s="11" cm="1">
         <f t="array" ref="I200">_xlfn.IFNA(_xlfn.IFS($D200&gt;=$B$206,$D200*0.15,AND($D200&lt;$B$206,$D200&gt;=$B$205),$D200*0.07,AND($D200&lt;$B$205,$D200&gt;=$B$204),$D200*0.03,AND($D200&lt;$B$204,$D200&gt;=$B$203),D200*0.01),0)</f>
         <v>5.65</v>
       </c>

</xml_diff>